<commit_message>
BR updates, with new Expected number
</commit_message>
<xml_diff>
--- a/plots_to_show/BR/final_metrics.xlsx
+++ b/plots_to_show/BR/final_metrics.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,22 +416,22 @@
         </is>
       </c>
       <c r="C2">
-        <v>8104.424187726412</v>
+        <v>11484.54150769252</v>
       </c>
       <c r="D2">
-        <v>40.44168098734507</v>
+        <v>25.05055481377521</v>
       </c>
       <c r="E2">
-        <v>6329.5676584957</v>
+        <v>8868.131248810469</v>
       </c>
       <c r="F2">
-        <v>37.50869182877114</v>
+        <v>21.73535765496148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -440,31 +440,31 @@
         </is>
       </c>
       <c r="C3">
-        <v>4568.132903589492</v>
+        <v>7329.351261883578</v>
       </c>
       <c r="D3">
-        <v>31.92565723429096</v>
+        <v>20.54423506440512</v>
       </c>
       <c r="E3">
-        <v>4263.003395833333</v>
+        <v>6857.531895833334</v>
       </c>
       <c r="F3">
-        <v>29.89145290491064</v>
+        <v>18.94458433570844</v>
       </c>
       <c r="G3">
-        <v>3923.707832935417</v>
+        <v>5995.919793907084</v>
       </c>
       <c r="H3">
-        <v>0.2083333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RS</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -473,49 +473,391 @@
         </is>
       </c>
       <c r="C4">
-        <v>4519.588375177575</v>
+        <v>7215.949265573547</v>
       </c>
       <c r="D4">
-        <v>37.73444381918399</v>
+        <v>20.43864114403762</v>
       </c>
       <c r="E4">
-        <v>4284.081691666667</v>
+        <v>6712.609825</v>
       </c>
       <c r="F4">
-        <v>34.99444065935269</v>
+        <v>17.89565582890354</v>
       </c>
       <c r="G4">
-        <v>3792.826712135</v>
+        <v>5940.490625765001</v>
       </c>
       <c r="H4">
-        <v>0.25</v>
+        <v>0.625</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bastos</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>5690.171660987475</v>
+      </c>
+      <c r="D5">
+        <v>14.24321709177373</v>
+      </c>
+      <c r="E5">
+        <v>5397.5625</v>
+      </c>
+      <c r="F5">
+        <v>13.15637387704677</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>RS</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>8104.424187726412</v>
+      </c>
+      <c r="D6">
+        <v>40.44168098734507</v>
+      </c>
+      <c r="E6">
+        <v>6329.5676584957</v>
+      </c>
+      <c r="F6">
+        <v>37.50869182877114</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ARABM</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>4486.419654327045</v>
+      </c>
+      <c r="D7">
+        <v>29.71708581109228</v>
+      </c>
+      <c r="E7">
+        <v>4186.94315</v>
+      </c>
+      <c r="F7">
+        <v>27.87180647166429</v>
+      </c>
+      <c r="G7">
+        <v>3804.940174281667</v>
+      </c>
+      <c r="H7">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="I7">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ARABMwGT</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>4306.349778019565</v>
+      </c>
+      <c r="D8">
+        <v>30.12556962316969</v>
+      </c>
+      <c r="E8">
+        <v>4074.276945833333</v>
+      </c>
+      <c r="F8">
+        <v>29.05932882587462</v>
+      </c>
+      <c r="G8">
+        <v>3631.572503907084</v>
+      </c>
+      <c r="H8">
+        <v>0.25</v>
+      </c>
+      <c r="I8">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RS</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Bastos</t>
         </is>
       </c>
-      <c r="C5">
+      <c r="C9">
         <v>3872.603633731065</v>
       </c>
-      <c r="D5">
+      <c r="D9">
         <v>25.10600316886911</v>
       </c>
-      <c r="E5">
+      <c r="E9">
         <v>3601.916666666667</v>
       </c>
-      <c r="F5">
+      <c r="F9">
         <v>24.21745359574475</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>11282.176059295</v>
+      </c>
+      <c r="D10">
+        <v>33.88616903808781</v>
+      </c>
+      <c r="E10">
+        <v>9046.618010075275</v>
+      </c>
+      <c r="F10">
+        <v>32.07223505271391</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ARABM</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>7175.025466313111</v>
+      </c>
+      <c r="D11">
+        <v>26.44259085286908</v>
+      </c>
+      <c r="E11">
+        <v>6662.606929166667</v>
+      </c>
+      <c r="F11">
+        <v>24.21966148458909</v>
+      </c>
+      <c r="G11">
+        <v>6028.18712075125</v>
+      </c>
+      <c r="H11">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="I11">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ARABMwGT</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>6977.156431230755</v>
+      </c>
+      <c r="D12">
+        <v>23.18352177633213</v>
+      </c>
+      <c r="E12">
+        <v>6605.0982125</v>
+      </c>
+      <c r="F12">
+        <v>22.40151803302255</v>
+      </c>
+      <c r="G12">
+        <v>5986.542579855417</v>
+      </c>
+      <c r="H12">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="I12">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SC</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bastos</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>7571.527352955327</v>
+      </c>
+      <c r="D13">
+        <v>26.42503346544768</v>
+      </c>
+      <c r="E13">
+        <v>7249.666666666667</v>
+      </c>
+      <c r="F13">
+        <v>24.68192918616597</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>GT</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>62798.26853839643</v>
+      </c>
+      <c r="D14">
+        <v>34.67147554185567</v>
+      </c>
+      <c r="E14">
+        <v>55360.37226797239</v>
+      </c>
+      <c r="F14">
+        <v>33.50512395722087</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ARABM</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>50254.56183357508</v>
+      </c>
+      <c r="D15">
+        <v>37.13364301222754</v>
+      </c>
+      <c r="E15">
+        <v>45067.97170416667</v>
+      </c>
+      <c r="F15">
+        <v>32.92768747019047</v>
+      </c>
+      <c r="G15">
+        <v>40019.49618830125</v>
+      </c>
+      <c r="H15">
+        <v>0.25</v>
+      </c>
+      <c r="I15">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ARABMwGT</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>49014.15604734916</v>
+      </c>
+      <c r="D16">
+        <v>32.53678946992844</v>
+      </c>
+      <c r="E16">
+        <v>45322.26379583334</v>
+      </c>
+      <c r="F16">
+        <v>30.2417805435602</v>
+      </c>
+      <c r="G16">
+        <v>39753.50108213459</v>
+      </c>
+      <c r="H16">
+        <v>0.25</v>
+      </c>
+      <c r="I16">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bastos</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>57132.55334683681</v>
+      </c>
+      <c r="D17">
+        <v>31.63492990547712</v>
+      </c>
+      <c r="E17">
+        <v>54985.20833333334</v>
+      </c>
+      <c r="F17">
+        <v>31.10286451291734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>